<commit_message>
add example file for CSR CropScan device
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_SpectrometerSystemCropScan.xlsx
+++ b/curator_data/examples/T3/CSRinT3_SpectrometerSystemCropScan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Spectrometer serial number</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Entrance slit aperture (um)</t>
-  </si>
-  <si>
-    <t>P50-2-UV</t>
   </si>
   <si>
     <t>The following information can be entered in the form. Information with a green background is required, others are optional.</t>
@@ -75,10 +72,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>barium sulfate</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Second-spectrometer serial number</t>
   </si>
   <si>
@@ -98,6 +91,9 @@
   </si>
   <si>
     <t>420</t>
+  </si>
+  <si>
+    <t>diffusing flashed white opal glass</t>
   </si>
 </sst>
 </file>
@@ -155,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +168,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -205,9 +207,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -215,6 +214,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -558,7 +560,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -571,52 +573,52 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>24</v>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="C4"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -631,7 +633,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -641,41 +643,39 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
+      <c r="B11"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:4">
       <c r="B15"/>

</xml_diff>